<commit_message>
SORTED TC101 and started to proced TC 102
</commit_message>
<xml_diff>
--- a/Testdata.xlsx
+++ b/Testdata.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TC101" sheetId="1" r:id="rId1"/>
-    <sheet name="TC102" sheetId="2" r:id="rId2"/>
+    <sheet name="TC102" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Username</t>
   </si>
@@ -27,6 +27,45 @@
   </si>
   <si>
     <t>Testing@123</t>
+  </si>
+  <si>
+    <t>No.of rooms</t>
+  </si>
+  <si>
+    <t>check in date</t>
+  </si>
+  <si>
+    <t>Check out date</t>
+  </si>
+  <si>
+    <t>2 - two</t>
+  </si>
+  <si>
+    <t>LOCATION</t>
+  </si>
+  <si>
+    <t>HOTELS</t>
+  </si>
+  <si>
+    <t>ROOM_TYPE</t>
+  </si>
+  <si>
+    <t>ADULTS PER ROOM</t>
+  </si>
+  <si>
+    <t>CHILD PER ROOM</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>Hotel Creek</t>
+  </si>
+  <si>
+    <t>1 - One</t>
+  </si>
+  <si>
+    <t>Standard</t>
   </si>
 </sst>
 </file>
@@ -71,9 +110,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -381,11 +421,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -413,12 +457,77 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2">
+        <v>45055</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45053</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>